<commit_message>
Update: Backup.xlsx File from Crowdin
</commit_message>
<xml_diff>
--- a/ja/Backup.xlsx
+++ b/ja/Backup.xlsx
@@ -1,21 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26026"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58E56EF9-DC96-4754-BD7E-CD995216AB74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </bookViews>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
-    <sheet name="Main" sheetId="1" r:id="rId1"/>
+    <sheet sheetId="1" name="Main" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="206">
   <si>
     <t>日本語</t>
   </si>
@@ -546,221 +542,115 @@
     <t>GMP</t>
   </si>
   <si>
+    <t>Coroner</t>
+  </si>
+  <si>
+    <t>検視官</t>
+  </si>
+  <si>
     <t>NoDeadBodies</t>
-    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>この付近に~r~死体~s~はありません。</t>
   </si>
   <si>
     <t>UnitRequested</t>
-    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>~b~{0}~s~の応援を要請しました。</t>
-    <rPh sb="10" eb="12">
-      <t>オウエン</t>
-    </rPh>
-    <rPh sb="13" eb="15">
-      <t>ヨウセイ</t>
-    </rPh>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>この付近に~r~死体~s~はありません。</t>
-    <rPh sb="2" eb="4">
-      <t>フキン</t>
-    </rPh>
-    <rPh sb="8" eb="10">
-      <t>シタイ</t>
-    </rPh>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Coroner</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>検視官</t>
-    <rPh sb="0" eb="3">
-      <t>ケンシカン</t>
-    </rPh>
-    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>CoronerCheckPls</t>
-    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>詳しい情報は~b~検視官レポート~s~を確認してください。</t>
-    <rPh sb="0" eb="1">
-      <t>クワ</t>
-    </rPh>
-    <rPh sb="3" eb="5">
-      <t>ジョウホウ</t>
-    </rPh>
-    <rPh sb="9" eb="12">
-      <t>ケンシカン</t>
-    </rPh>
-    <rPh sb="20" eb="22">
-      <t>カクニン</t>
-    </rPh>
-    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>CoronerBye</t>
-    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>それではいい一日を!</t>
-    <rPh sb="6" eb="8">
-      <t>イチニチ</t>
-    </rPh>
-    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>TeleportUnit</t>
-    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>{0}で応援を近くにテレポートさせます。</t>
-    <rPh sb="4" eb="6">
-      <t>オウエン</t>
-    </rPh>
-    <rPh sb="7" eb="8">
-      <t>チカ</t>
-    </rPh>
-    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>CoronerMenu</t>
-    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>検視官メニュー</t>
-    <rPh sb="0" eb="3">
-      <t>ケンシカン</t>
-    </rPh>
-    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>CoronerReport</t>
+  </si>
+  <si>
+    <t>検視官レポート</t>
   </si>
   <si>
     <t>CoronerReportCount</t>
-    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>検視官レポート数: {0}</t>
-    <rPh sb="0" eb="3">
-      <t>ケンシカン</t>
-    </rPh>
-    <rPh sb="7" eb="8">
-      <t>スウ</t>
-    </rPh>
-    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>NoData</t>
+  </si>
+  <si>
+    <t>データなし</t>
   </si>
   <si>
     <t>Name</t>
-    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>名前</t>
-    <rPh sb="0" eb="2">
-      <t>ナマエ</t>
-    </rPh>
-    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>Sex</t>
-    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>性別</t>
-    <rPh sb="0" eb="2">
-      <t>セイベツ</t>
-    </rPh>
-    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>CauseOfDeath</t>
-    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>死因</t>
-    <rPh sb="0" eb="2">
-      <t>シイン</t>
-    </rPh>
-    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>DiedDay</t>
-    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>死亡日</t>
-    <rPh sb="0" eb="2">
-      <t>シボウ</t>
-    </rPh>
-    <rPh sb="2" eb="3">
-      <t>ヒ</t>
-    </rPh>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>NoData</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>データなし</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>CoronerReport</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>検視官レポート</t>
-    <rPh sb="0" eb="3">
-      <t>ケンシカン</t>
-    </rPh>
-    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>BackupVehicle</t>
-    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>応援車両</t>
-    <rPh sb="0" eb="2">
-      <t>オウエン</t>
-    </rPh>
-    <rPh sb="2" eb="4">
-      <t>シャリョウ</t>
-    </rPh>
-    <phoneticPr fontId="2"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="ＭＳ Ｐゴシック"/>
       <family val="2"/>
       <scheme val="minor"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
     <font>
+      <charset val="128"/>
+      <color theme="1"/>
+      <family val="2"/>
+      <scheme val="minor"/>
       <sz val="11"/>
-      <color theme="1"/>
       <name val="ＭＳ Ｐゴシック"/>
-      <family val="2"/>
-      <charset val="128"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="6"/>
-      <name val="ＭＳ Ｐゴシック"/>
-      <family val="3"/>
-      <charset val="128"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -790,7 +680,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="標準" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1126,20 +1016,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V43"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="22.625" customWidth="1"/>
     <col min="2" max="18" width="30.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="1" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1204,7 +1089,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:22" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" ht="13.5" customHeight="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -1230,7 +1115,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:22" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" ht="13.5" customHeight="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -1256,7 +1141,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:22" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" ht="13.5" customHeight="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>36</v>
       </c>
@@ -1282,7 +1167,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:22" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" ht="13.5" customHeight="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>42</v>
       </c>
@@ -1308,7 +1193,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:22" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" ht="13.5" customHeight="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>48</v>
       </c>
@@ -1334,7 +1219,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:22" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" ht="13.5" customHeight="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>54</v>
       </c>
@@ -1360,7 +1245,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:22" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" ht="13.5" customHeight="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>60</v>
       </c>
@@ -1386,7 +1271,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="9" spans="1:22" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" ht="13.5" customHeight="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>68</v>
       </c>
@@ -1412,7 +1297,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="10" spans="1:22" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" ht="13.5" customHeight="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>76</v>
       </c>
@@ -1438,7 +1323,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="11" spans="1:22" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" ht="13.5" customHeight="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>84</v>
       </c>
@@ -1464,16 +1349,13 @@
         <v>91</v>
       </c>
     </row>
-    <row r="13" spans="1:22" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" ht="13.5" customHeight="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>92</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="E13" t="s">
-        <v>92</v>
-      </c>
       <c r="H13" t="s">
         <v>94</v>
       </c>
@@ -1490,16 +1372,13 @@
         <v>98</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>99</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="E14" t="s">
-        <v>99</v>
-      </c>
       <c r="H14" t="s">
         <v>101</v>
       </c>
@@ -1516,7 +1395,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>106</v>
       </c>
@@ -1542,16 +1421,13 @@
         <v>113</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>114</v>
       </c>
       <c r="B16" t="s">
         <v>115</v>
       </c>
-      <c r="E16" t="s">
-        <v>114</v>
-      </c>
       <c r="H16" t="s">
         <v>116</v>
       </c>
@@ -1568,7 +1444,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>121</v>
       </c>
@@ -1594,7 +1470,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>129</v>
       </c>
@@ -1620,7 +1496,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>137</v>
       </c>
@@ -1646,7 +1522,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>145</v>
       </c>
@@ -1672,7 +1548,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>153</v>
       </c>
@@ -1698,7 +1574,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>161</v>
       </c>
@@ -1724,7 +1600,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>168</v>
       </c>
@@ -1750,31 +1626,31 @@
         <v>175</v>
       </c>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B26" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.15">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B27" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="B28" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.15">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>182</v>
       </c>
@@ -1782,7 +1658,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>184</v>
       </c>
@@ -1790,7 +1666,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>186</v>
       </c>
@@ -1798,7 +1674,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>188</v>
       </c>
@@ -1806,63 +1682,63 @@
         <v>189</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>190</v>
+      </c>
+      <c r="B34" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>192</v>
+      </c>
+      <c r="B35" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>194</v>
+      </c>
+      <c r="B36" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>196</v>
+      </c>
+      <c r="B38" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>198</v>
+      </c>
+      <c r="B39" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>200</v>
+      </c>
+      <c r="B40" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>202</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B41" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A35" t="s">
-        <v>190</v>
-      </c>
-      <c r="B35" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A36" t="s">
-        <v>200</v>
-      </c>
-      <c r="B36" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A38" t="s">
-        <v>192</v>
-      </c>
-      <c r="B38" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A39" t="s">
-        <v>194</v>
-      </c>
-      <c r="B39" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A40" t="s">
-        <v>196</v>
-      </c>
-      <c r="B40" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A41" t="s">
-        <v>198</v>
-      </c>
-      <c r="B41" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>204</v>
       </c>
@@ -1871,8 +1747,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="4294967295" verticalDpi="4294967295"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update: %original_file_name% File from Crowdin
</commit_message>
<xml_diff>
--- a/ja/Backup.xlsx
+++ b/ja/Backup.xlsx
@@ -1,17 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26026"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58E56EF9-DC96-4754-BD7E-CD995216AB74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet sheetId="1" name="Main" state="visible" r:id="rId4"/>
+    <sheet name="Main" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="206">
   <si>
     <t>日本語</t>
   </si>
@@ -542,115 +546,221 @@
     <t>GMP</t>
   </si>
   <si>
+    <t>NoDeadBodies</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>UnitRequested</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>~b~{0}~s~の応援を要請しました。</t>
+    <rPh sb="10" eb="12">
+      <t>オウエン</t>
+    </rPh>
+    <rPh sb="13" eb="15">
+      <t>ヨウセイ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>この付近に~r~死体~s~はありません。</t>
+    <rPh sb="2" eb="4">
+      <t>フキン</t>
+    </rPh>
+    <rPh sb="8" eb="10">
+      <t>シタイ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
     <t>Coroner</t>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>検視官</t>
-  </si>
-  <si>
-    <t>NoDeadBodies</t>
-  </si>
-  <si>
-    <t>この付近に~r~死体~s~はありません。</t>
-  </si>
-  <si>
-    <t>UnitRequested</t>
-  </si>
-  <si>
-    <t>~b~{0}~s~の応援を要請しました。</t>
+    <rPh sb="0" eb="3">
+      <t>ケンシカン</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>CoronerCheckPls</t>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>詳しい情報は~b~検視官レポート~s~を確認してください。</t>
+    <rPh sb="0" eb="1">
+      <t>クワ</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>ジョウホウ</t>
+    </rPh>
+    <rPh sb="9" eb="12">
+      <t>ケンシカン</t>
+    </rPh>
+    <rPh sb="20" eb="22">
+      <t>カクニン</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>CoronerBye</t>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>それではいい一日を!</t>
+    <rPh sb="6" eb="8">
+      <t>イチニチ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>TeleportUnit</t>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>{0}で応援を近くにテレポートさせます。</t>
+    <rPh sb="4" eb="6">
+      <t>オウエン</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>チカ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>CoronerMenu</t>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>検視官メニュー</t>
+    <rPh sb="0" eb="3">
+      <t>ケンシカン</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>CoronerReportCount</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>検視官レポート数: {0}</t>
+    <rPh sb="0" eb="3">
+      <t>ケンシカン</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>スウ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Name</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>名前</t>
+    <rPh sb="0" eb="2">
+      <t>ナマエ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Sex</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>性別</t>
+    <rPh sb="0" eb="2">
+      <t>セイベツ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>CauseOfDeath</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>死因</t>
+    <rPh sb="0" eb="2">
+      <t>シイン</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>DiedDay</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>死亡日</t>
+    <rPh sb="0" eb="2">
+      <t>シボウ</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>ヒ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>NoData</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>データなし</t>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>CoronerReport</t>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>検視官レポート</t>
-  </si>
-  <si>
-    <t>CoronerReportCount</t>
-  </si>
-  <si>
-    <t>検視官レポート数: {0}</t>
-  </si>
-  <si>
-    <t>NoData</t>
-  </si>
-  <si>
-    <t>データなし</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>名前</t>
-  </si>
-  <si>
-    <t>Sex</t>
-  </si>
-  <si>
-    <t>性別</t>
-  </si>
-  <si>
-    <t>CauseOfDeath</t>
-  </si>
-  <si>
-    <t>死因</t>
-  </si>
-  <si>
-    <t>DiedDay</t>
-  </si>
-  <si>
-    <t>死亡日</t>
+    <rPh sb="0" eb="3">
+      <t>ケンシカン</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>BackupVehicle</t>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>応援車両</t>
+    <rPh sb="0" eb="2">
+      <t>オウエン</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>シャリョウ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="ＭＳ Ｐゴシック"/>
       <family val="2"/>
       <scheme val="minor"/>
-      <sz val="11"/>
-      <name val="Calibri"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="2"/>
       <charset val="128"/>
-      <color theme="1"/>
-      <family val="2"/>
       <scheme val="minor"/>
-      <sz val="11"/>
+    </font>
+    <font>
+      <sz val="6"/>
       <name val="ＭＳ Ｐゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -680,7 +790,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="標準" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1016,15 +1126,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V43"/>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A44" sqref="A44"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="22.625" customWidth="1"/>
     <col min="2" max="18" width="30.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.15">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1089,7 +1204,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" ht="13.5" customHeight="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -1115,7 +1230,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" ht="13.5" customHeight="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -1141,7 +1256,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" ht="13.5" customHeight="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>36</v>
       </c>
@@ -1167,7 +1282,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" ht="13.5" customHeight="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>42</v>
       </c>
@@ -1193,7 +1308,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="6" ht="13.5" customHeight="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>48</v>
       </c>
@@ -1219,7 +1334,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" ht="13.5" customHeight="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>54</v>
       </c>
@@ -1245,7 +1360,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" ht="13.5" customHeight="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>60</v>
       </c>
@@ -1271,7 +1386,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="9" ht="13.5" customHeight="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>68</v>
       </c>
@@ -1297,7 +1412,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="10" ht="13.5" customHeight="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>76</v>
       </c>
@@ -1323,7 +1438,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="11" ht="13.5" customHeight="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>84</v>
       </c>
@@ -1349,13 +1464,16 @@
         <v>91</v>
       </c>
     </row>
-    <row r="13" ht="13.5" customHeight="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:22" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>92</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>93</v>
       </c>
+      <c r="E13" t="s">
+        <v>92</v>
+      </c>
       <c r="H13" t="s">
         <v>94</v>
       </c>
@@ -1372,13 +1490,16 @@
         <v>98</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>99</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>100</v>
       </c>
+      <c r="E14" t="s">
+        <v>99</v>
+      </c>
       <c r="H14" t="s">
         <v>101</v>
       </c>
@@ -1395,7 +1516,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>106</v>
       </c>
@@ -1421,13 +1542,16 @@
         <v>113</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>114</v>
       </c>
       <c r="B16" t="s">
         <v>115</v>
       </c>
+      <c r="E16" t="s">
+        <v>114</v>
+      </c>
       <c r="H16" t="s">
         <v>116</v>
       </c>
@@ -1444,7 +1568,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>121</v>
       </c>
@@ -1470,7 +1594,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>129</v>
       </c>
@@ -1496,7 +1620,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>137</v>
       </c>
@@ -1522,7 +1646,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
         <v>145</v>
       </c>
@@ -1548,7 +1672,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
         <v>153</v>
       </c>
@@ -1574,7 +1698,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
         <v>161</v>
       </c>
@@ -1600,7 +1724,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
         <v>168</v>
       </c>
@@ -1626,31 +1750,31 @@
         <v>175</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
+        <v>180</v>
+      </c>
+      <c r="B26" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.15">
+      <c r="A27" t="s">
         <v>176</v>
-      </c>
-      <c r="B26" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>178</v>
       </c>
       <c r="B27" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B28" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
         <v>182</v>
       </c>
@@ -1658,7 +1782,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
         <v>184</v>
       </c>
@@ -1666,7 +1790,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
         <v>186</v>
       </c>
@@ -1674,7 +1798,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
         <v>188</v>
       </c>
@@ -1682,63 +1806,63 @@
         <v>189</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
+        <v>202</v>
+      </c>
+      <c r="B34" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A35" t="s">
         <v>190</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B35" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A36" t="s">
+        <v>200</v>
+      </c>
+      <c r="B36" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A38" t="s">
         <v>192</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B38" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A39" t="s">
         <v>194</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B39" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A40" t="s">
         <v>196</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B40" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A41" t="s">
         <v>198</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B41" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>200</v>
-      </c>
-      <c r="B40" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>202</v>
-      </c>
-      <c r="B41" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A43" t="s">
         <v>204</v>
       </c>
@@ -1747,7 +1871,8 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
+  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="4294967295" verticalDpi="4294967295"/>
 </worksheet>
 </file>
</xml_diff>